<commit_message>
Versions 1.1,Add Windows Service and log func.
</commit_message>
<xml_diff>
--- a/Conf/S7_PLC15.Main.xlsx
+++ b/Conf/S7_PLC15.Main.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="208">
   <si>
     <t>Tag Name</t>
   </si>
@@ -82,6 +82,42 @@
     <t>Conveyor Inclined Carousal Dep_Carousel</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_DC101_DC101_ES01_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB5</t>
+  </si>
+  <si>
+    <t>Conveyor ESTOP E_stop_Control_Station</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC101_DC101_ES02_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB6</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC101_DC101_ES03_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB7</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC101_DC101_ES04_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB8</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC101_DC101_IOB_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB581</t>
+  </si>
+  <si>
+    <t>Conveyor IOB IOB</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_DC101_DC101_SIGNAL_1</t>
   </si>
   <si>
@@ -97,6 +133,36 @@
     <t>DB200.DBB452</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_DC103_DC103_ES01_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB9</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC103_DC103_ES02_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB10</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC103_DC103_ES03_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB11</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC103_DC103_ES04_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB12</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DC103_DC103_IOB_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB582</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_DC103_DC103_SIGNAL_1</t>
   </si>
   <si>
@@ -172,6 +238,18 @@
     <t>DB200.DBD174</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_DL11_DL11_BC001_ES_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB1</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DL11_DL11_BC001_IOB_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB578</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_DL11_PC002_CM</t>
   </si>
   <si>
@@ -265,6 +343,30 @@
     <t>DB200.DBD286</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_DL12_DL12_BC001_ES_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB2</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DL12_DL12_BC001_IOB_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB579</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DL12_DL12_BC003_ES_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB3</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DL12_DL12_BC003_IOB_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB580</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_DL12_PC004_CM</t>
   </si>
   <si>
@@ -295,6 +397,21 @@
     <t>DB200.DBD258</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_DL12_TTS01_DPDP01_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB583</t>
+  </si>
+  <si>
+    <t>Conveyor DPC DPC</t>
+  </si>
+  <si>
+    <t>CRISBELT_PLC15_DL12_TTS01_DPDP02_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB200.DBB584</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_DT01_BC002_CM</t>
   </si>
   <si>
@@ -418,6 +535,12 @@
     <t>DB200.DBD440</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_MCC01_FCC01_ES_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB0</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_MCC01_FCC01_SIGNAL_1</t>
   </si>
   <si>
@@ -433,6 +556,12 @@
     <t>DB200.DBD18</t>
   </si>
   <si>
+    <t>CRISBELT_PLC15_MCC01_FCC02_ES_SIGNAL_1</t>
+  </si>
+  <si>
+    <t>DB30.DBB4</t>
+  </si>
+  <si>
     <t>CRISBELT_PLC15_MCC01_FCC02_SIGNAL_1</t>
   </si>
   <si>
@@ -490,7 +619,7 @@
     <t>DB200.DBW86</t>
   </si>
   <si>
-    <t>CRISBELT_PLC15_PLC_PLC18_SIGNAL_1</t>
+    <t>CRISBELT_PLC15_PLC_PLC15_SIGNAL_1</t>
   </si>
   <si>
     <t>DB200.DBW4</t>
@@ -499,16 +628,13 @@
     <t>Conveyor PLC PLC</t>
   </si>
   <si>
-    <t>CRISBELT_PLC15_SYSTEM_KAL_DEVICE1_SIGNAL_1</t>
+    <t>CRISBELT_PLC15_SYSTEM_KAL_DEVICE2_SIGNAL_1</t>
   </si>
   <si>
     <t>DB200.DBW0</t>
   </si>
   <si>
     <t>Conveyor System Signals_Only</t>
-  </si>
-  <si>
-    <t>CRISBELT_PLC15_SYSTEM_KAL_DEVICE2_SIGNAL_1</t>
   </si>
   <si>
     <t>CRISBELT_PLC15_SYSTEM_KAL_MAIN_SIGNAL_1</t>
@@ -1340,7 +1466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1430,19 +1556,19 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="P3" t="s">
         <v>24</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -1465,7 +1591,7 @@
         <v>100</v>
       </c>
       <c r="P4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -1476,19 +1602,19 @@
         <v>28</v>
       </c>
       <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="P5" t="s">
         <v>24</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="P5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -1511,30 +1637,30 @@
         <v>100</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="P7" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-      <c r="P7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1545,7 +1671,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1557,7 +1683,7 @@
         <v>100</v>
       </c>
       <c r="P8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1568,7 +1694,7 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1580,7 +1706,7 @@
         <v>100</v>
       </c>
       <c r="P9" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1603,7 +1729,7 @@
         <v>100</v>
       </c>
       <c r="P10" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1614,19 +1740,19 @@
         <v>42</v>
       </c>
       <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="P11" t="s">
         <v>24</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11">
-        <v>100</v>
-      </c>
-      <c r="P11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1649,7 +1775,7 @@
         <v>100</v>
       </c>
       <c r="P12" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1660,19 +1786,19 @@
         <v>46</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="P13" t="s">
         <v>24</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
-      <c r="P13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -1695,18 +1821,18 @@
         <v>100</v>
       </c>
       <c r="P14" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1718,41 +1844,41 @@
         <v>100</v>
       </c>
       <c r="P15" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+      <c r="P16" t="s">
         <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16">
-        <v>100</v>
-      </c>
-      <c r="P16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="B17" t="s">
-        <v>56</v>
-      </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1764,30 +1890,30 @@
         <v>100</v>
       </c>
       <c r="P17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="P18" t="s">
         <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18">
-        <v>100</v>
-      </c>
-      <c r="P18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -1798,7 +1924,7 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -1810,7 +1936,7 @@
         <v>100</v>
       </c>
       <c r="P19" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -1833,18 +1959,18 @@
         <v>100</v>
       </c>
       <c r="P20" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1856,16 +1982,16 @@
         <v>100</v>
       </c>
       <c r="P21" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
         <v>66</v>
       </c>
-      <c r="B22" t="s">
-        <v>67</v>
-      </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
@@ -1879,18 +2005,18 @@
         <v>100</v>
       </c>
       <c r="P22" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1902,41 +2028,41 @@
         <v>100</v>
       </c>
       <c r="P23" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>100</v>
+      </c>
+      <c r="P24" t="s">
         <v>71</v>
-      </c>
-      <c r="B24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24">
-        <v>100</v>
-      </c>
-      <c r="P24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1948,16 +2074,16 @@
         <v>100</v>
       </c>
       <c r="P25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
         <v>75</v>
       </c>
-      <c r="B26" t="s">
-        <v>76</v>
-      </c>
       <c r="C26" t="s">
         <v>19</v>
       </c>
@@ -1971,18 +2097,18 @@
         <v>100</v>
       </c>
       <c r="P26" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1994,30 +2120,30 @@
         <v>100</v>
       </c>
       <c r="P27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>100</v>
+      </c>
+      <c r="P28" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28">
-        <v>100</v>
-      </c>
-      <c r="P28" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -2028,7 +2154,7 @@
         <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2040,7 +2166,7 @@
         <v>100</v>
       </c>
       <c r="P29" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -2063,18 +2189,18 @@
         <v>100</v>
       </c>
       <c r="P30" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
         <v>86</v>
       </c>
-      <c r="B31" t="s">
-        <v>87</v>
-      </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2086,41 +2212,41 @@
         <v>100</v>
       </c>
       <c r="P31" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
         <v>88</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>100</v>
+      </c>
+      <c r="P32" t="s">
         <v>89</v>
-      </c>
-      <c r="C32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32">
-        <v>100</v>
-      </c>
-      <c r="P32" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
         <v>91</v>
       </c>
-      <c r="B33" t="s">
-        <v>92</v>
-      </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2132,41 +2258,41 @@
         <v>100</v>
       </c>
       <c r="P33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
         <v>93</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>100</v>
+      </c>
+      <c r="P34" t="s">
         <v>94</v>
-      </c>
-      <c r="C34" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34">
-        <v>100</v>
-      </c>
-      <c r="P34" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" t="s">
         <v>96</v>
       </c>
-      <c r="B35" t="s">
-        <v>97</v>
-      </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D35">
         <v>1</v>
@@ -2178,16 +2304,16 @@
         <v>100</v>
       </c>
       <c r="P35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" t="s">
         <v>98</v>
       </c>
-      <c r="B36" t="s">
-        <v>99</v>
-      </c>
       <c r="C36" t="s">
         <v>19</v>
       </c>
@@ -2201,18 +2327,18 @@
         <v>100</v>
       </c>
       <c r="P36" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -2224,16 +2350,16 @@
         <v>100</v>
       </c>
       <c r="P37" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B38" t="s">
         <v>102</v>
       </c>
-      <c r="B38" t="s">
-        <v>103</v>
-      </c>
       <c r="C38" t="s">
         <v>19</v>
       </c>
@@ -2247,18 +2373,18 @@
         <v>100</v>
       </c>
       <c r="P38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
         <v>104</v>
       </c>
-      <c r="B39" t="s">
-        <v>105</v>
-      </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D39">
         <v>1</v>
@@ -2270,16 +2396,16 @@
         <v>100</v>
       </c>
       <c r="P39" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
         <v>106</v>
       </c>
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
       <c r="C40" t="s">
         <v>19</v>
       </c>
@@ -2293,18 +2419,18 @@
         <v>100</v>
       </c>
       <c r="P40" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s">
         <v>108</v>
       </c>
-      <c r="B41" t="s">
-        <v>109</v>
-      </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2316,16 +2442,16 @@
         <v>100</v>
       </c>
       <c r="P41" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" t="s">
         <v>110</v>
       </c>
-      <c r="B42" t="s">
-        <v>111</v>
-      </c>
       <c r="C42" t="s">
         <v>19</v>
       </c>
@@ -2339,18 +2465,18 @@
         <v>100</v>
       </c>
       <c r="P42" t="s">
-        <v>95</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
         <v>112</v>
       </c>
-      <c r="B43" t="s">
-        <v>113</v>
-      </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2362,16 +2488,16 @@
         <v>100</v>
       </c>
       <c r="P43" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" t="s">
         <v>114</v>
       </c>
-      <c r="B44" t="s">
-        <v>115</v>
-      </c>
       <c r="C44" t="s">
         <v>19</v>
       </c>
@@ -2385,18 +2511,18 @@
         <v>100</v>
       </c>
       <c r="P44" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
         <v>116</v>
       </c>
-      <c r="B45" t="s">
-        <v>117</v>
-      </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2408,30 +2534,30 @@
         <v>100</v>
       </c>
       <c r="P45" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" t="s">
         <v>118</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+      <c r="P46" t="s">
         <v>119</v>
-      </c>
-      <c r="C46" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46">
-        <v>100</v>
-      </c>
-      <c r="P46" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -2442,7 +2568,7 @@
         <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2454,7 +2580,7 @@
         <v>100</v>
       </c>
       <c r="P47" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -2477,38 +2603,38 @@
         <v>100</v>
       </c>
       <c r="P48" t="s">
-        <v>36</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="P49" t="s">
         <v>124</v>
-      </c>
-      <c r="B49" t="s">
-        <v>125</v>
-      </c>
-      <c r="C49" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49">
-        <v>100</v>
-      </c>
-      <c r="P49" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B50" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
         <v>19</v>
@@ -2523,38 +2649,38 @@
         <v>100</v>
       </c>
       <c r="P50" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
+        <v>131</v>
+      </c>
+      <c r="C51" t="s">
+        <v>19</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51">
+        <v>100</v>
+      </c>
+      <c r="P51" t="s">
         <v>129</v>
-      </c>
-      <c r="C51" t="s">
-        <v>24</v>
-      </c>
-      <c r="D51">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51">
-        <v>100</v>
-      </c>
-      <c r="P51" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C52" t="s">
         <v>19</v>
@@ -2569,18 +2695,18 @@
         <v>100</v>
       </c>
       <c r="P52" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D53">
         <v>1</v>
@@ -2592,18 +2718,18 @@
         <v>100</v>
       </c>
       <c r="P53" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B54" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D54">
         <v>1</v>
@@ -2615,18 +2741,18 @@
         <v>100</v>
       </c>
       <c r="P54" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B55" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D55">
         <v>1</v>
@@ -2638,18 +2764,18 @@
         <v>100</v>
       </c>
       <c r="P55" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2661,18 +2787,18 @@
         <v>100</v>
       </c>
       <c r="P56" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -2684,18 +2810,18 @@
         <v>100</v>
       </c>
       <c r="P57" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C58" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -2707,7 +2833,7 @@
         <v>100</v>
       </c>
       <c r="P58" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.3">
@@ -2718,7 +2844,7 @@
         <v>148</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -2730,7 +2856,7 @@
         <v>100</v>
       </c>
       <c r="P59" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
@@ -2741,7 +2867,7 @@
         <v>150</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2753,18 +2879,18 @@
         <v>100</v>
       </c>
       <c r="P60" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>151</v>
+      </c>
+      <c r="B61" t="s">
         <v>152</v>
       </c>
-      <c r="B61" t="s">
-        <v>153</v>
-      </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2776,18 +2902,18 @@
         <v>100</v>
       </c>
       <c r="P61" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" t="s">
         <v>154</v>
       </c>
-      <c r="B62" t="s">
-        <v>155</v>
-      </c>
       <c r="C62" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2799,18 +2925,18 @@
         <v>100</v>
       </c>
       <c r="P62" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" t="s">
         <v>156</v>
       </c>
-      <c r="B63" t="s">
-        <v>157</v>
-      </c>
       <c r="C63" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2822,18 +2948,18 @@
         <v>100</v>
       </c>
       <c r="P63" t="s">
-        <v>146</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>157</v>
+      </c>
+      <c r="B64" t="s">
         <v>158</v>
       </c>
-      <c r="B64" t="s">
-        <v>159</v>
-      </c>
       <c r="C64" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -2845,18 +2971,18 @@
         <v>100</v>
       </c>
       <c r="P64" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2868,18 +2994,18 @@
         <v>100</v>
       </c>
       <c r="P65" t="s">
-        <v>163</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
         <v>162</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2891,30 +3017,467 @@
         <v>100</v>
       </c>
       <c r="P66" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67">
+        <v>100</v>
+      </c>
+      <c r="P67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>165</v>
       </c>
-      <c r="B67" t="s">
-        <v>162</v>
-      </c>
-      <c r="C67" t="s">
-        <v>145</v>
-      </c>
-      <c r="D67">
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67">
-        <v>100</v>
-      </c>
-      <c r="P67" t="s">
-        <v>163</v>
+      <c r="B68" t="s">
+        <v>166</v>
+      </c>
+      <c r="C68" t="s">
+        <v>19</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68">
+        <v>100</v>
+      </c>
+      <c r="P68" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" t="s">
+        <v>168</v>
+      </c>
+      <c r="C69" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69">
+        <v>100</v>
+      </c>
+      <c r="P69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>169</v>
+      </c>
+      <c r="B70" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70">
+        <v>100</v>
+      </c>
+      <c r="P70" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>171</v>
+      </c>
+      <c r="B71" t="s">
+        <v>172</v>
+      </c>
+      <c r="C71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71">
+        <v>100</v>
+      </c>
+      <c r="P71" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" t="s">
+        <v>174</v>
+      </c>
+      <c r="C72" t="s">
+        <v>19</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72">
+        <v>100</v>
+      </c>
+      <c r="P72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>175</v>
+      </c>
+      <c r="B73" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73">
+        <v>100</v>
+      </c>
+      <c r="P73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>178</v>
+      </c>
+      <c r="B74" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74">
+        <v>100</v>
+      </c>
+      <c r="P74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B75" t="s">
+        <v>181</v>
+      </c>
+      <c r="C75" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>20</v>
+      </c>
+      <c r="F75">
+        <v>100</v>
+      </c>
+      <c r="P75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>182</v>
+      </c>
+      <c r="B76" t="s">
+        <v>183</v>
+      </c>
+      <c r="C76" t="s">
+        <v>36</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76">
+        <v>100</v>
+      </c>
+      <c r="P76" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>184</v>
+      </c>
+      <c r="B77" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>20</v>
+      </c>
+      <c r="F77">
+        <v>100</v>
+      </c>
+      <c r="P77" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>186</v>
+      </c>
+      <c r="B78" t="s">
+        <v>187</v>
+      </c>
+      <c r="C78" t="s">
+        <v>188</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>20</v>
+      </c>
+      <c r="F78">
+        <v>100</v>
+      </c>
+      <c r="P78" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>190</v>
+      </c>
+      <c r="B79" t="s">
+        <v>191</v>
+      </c>
+      <c r="C79" t="s">
+        <v>188</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79">
+        <v>100</v>
+      </c>
+      <c r="P79" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" t="s">
+        <v>193</v>
+      </c>
+      <c r="C80" t="s">
+        <v>36</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>20</v>
+      </c>
+      <c r="F80">
+        <v>100</v>
+      </c>
+      <c r="P80" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>195</v>
+      </c>
+      <c r="B81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" t="s">
+        <v>36</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F81">
+        <v>100</v>
+      </c>
+      <c r="P81" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>197</v>
+      </c>
+      <c r="B82" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" t="s">
+        <v>188</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>20</v>
+      </c>
+      <c r="F82">
+        <v>100</v>
+      </c>
+      <c r="P82" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>199</v>
+      </c>
+      <c r="B83" t="s">
+        <v>200</v>
+      </c>
+      <c r="C83" t="s">
+        <v>188</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>20</v>
+      </c>
+      <c r="F83">
+        <v>100</v>
+      </c>
+      <c r="P83" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>201</v>
+      </c>
+      <c r="B84" t="s">
+        <v>202</v>
+      </c>
+      <c r="C84" t="s">
+        <v>188</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>20</v>
+      </c>
+      <c r="F84">
+        <v>100</v>
+      </c>
+      <c r="P84" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>204</v>
+      </c>
+      <c r="B85" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" t="s">
+        <v>188</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>20</v>
+      </c>
+      <c r="F85">
+        <v>100</v>
+      </c>
+      <c r="P85" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>207</v>
+      </c>
+      <c r="B86" t="s">
+        <v>205</v>
+      </c>
+      <c r="C86" t="s">
+        <v>188</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>20</v>
+      </c>
+      <c r="F86">
+        <v>100</v>
+      </c>
+      <c r="P86" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>